<commit_message>
Added email settings change in changing a role, Fixed a bug in userpagesearch.
</commit_message>
<xml_diff>
--- a/skrum_docs/04_SpecificDesign/26_Setting(User)_ユーザ設定画面仕様書_20170713.xlsx
+++ b/skrum_docs/04_SpecificDesign/26_Setting(User)_ユーザ設定画面仕様書_20170713.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="1020" yWindow="460" windowWidth="27780" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ユーザ招待" sheetId="1" r:id="rId1"/>
@@ -1730,8 +1730,8 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1028700</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1741,12 +1741,12 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8343900" y="647700"/>
-          <a:ext cx="5118100" cy="2019300"/>
+          <a:ext cx="5118100" cy="2324100"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -65012"/>
-            <a:gd name="adj2" fmla="val 86596"/>
+            <a:gd name="adj1" fmla="val -52853"/>
+            <a:gd name="adj2" fmla="val 72935"/>
           </a:avLst>
         </a:prstGeom>
         <a:solidFill>
@@ -1801,16 +1801,13 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800"/>
-            <a:t>v1/users/pagesearch.json?q=</a:t>
+            <a:t>v1/users/pagesearch.json?p=1&amp;q=</a:t>
           </a:r>
           <a:r>
             <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1800"/>
             <a:t>田</a:t>
           </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800"/>
-            <a:t>&amp;p=1</a:t>
-          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800"/>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -1822,6 +1819,33 @@
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800"/>
             <a:t>"p" = page</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800"/>
+            <a:t>"q" is not required.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>

</xml_diff>